<commit_message>
received  feedback from friend and figured out a way to sort the courses to make it easy to read and now it's sorted Alphabetically by Course.
</commit_message>
<xml_diff>
--- a/GradeDistributionsDB/Fall2015/Output/Fall2015 MD.xlsx
+++ b/GradeDistributionsDB/Fall2015/Output/Fall2015 MD.xlsx
@@ -25,19 +25,19 @@
     <t>GPA</t>
   </si>
   <si>
-    <t># of A's</t>
-  </si>
-  <si>
-    <t># of B's</t>
-  </si>
-  <si>
-    <t># of C's</t>
-  </si>
-  <si>
-    <t># of D's</t>
-  </si>
-  <si>
-    <t># of F's</t>
+    <t>% of A's</t>
+  </si>
+  <si>
+    <t>% of B's</t>
+  </si>
+  <si>
+    <t>% of C's</t>
+  </si>
+  <si>
+    <t>% of D's</t>
+  </si>
+  <si>
+    <t>% of F's</t>
   </si>
   <si>
     <t>EDHP-500</t>
@@ -55,18 +55,24 @@
     <t>0.00%</t>
   </si>
   <si>
+    <t>HCPI-555</t>
+  </si>
+  <si>
+    <t>MCCANN A</t>
+  </si>
+  <si>
+    <t>80.00%</t>
+  </si>
+  <si>
+    <t>20.00%</t>
+  </si>
+  <si>
     <t>MPHY-601</t>
   </si>
   <si>
     <t>ZHANG S</t>
   </si>
   <si>
-    <t>80.00%</t>
-  </si>
-  <si>
-    <t>20.00%</t>
-  </si>
-  <si>
     <t>MSCI-601</t>
   </si>
   <si>
@@ -101,12 +107,6 @@
   </si>
   <si>
     <t>COLLEGE T</t>
-  </si>
-  <si>
-    <t>HCPI-555</t>
-  </si>
-  <si>
-    <t>MCCANN A</t>
   </si>
 </sst>
 </file>
@@ -543,101 +543,101 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="n">
         <v>3.111</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="B10" t="s">
+      <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="n">
-        <v>3.222</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>25</v>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.222</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="n">
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="n">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="n">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
         <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -645,13 +645,13 @@
         <v>30</v>
       </c>
       <c r="C17" t="n">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>

</xml_diff>